<commit_message>
update to Dans spreadsheet
</commit_message>
<xml_diff>
--- a/projects/audit662.xlsx
+++ b/projects/audit662.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="60" windowWidth="2964" windowHeight="9048" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="16800" yWindow="60" windowWidth="2964" windowHeight="9048" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -3783,11 +3783,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1421">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5545,7 +5545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6072,8 +6072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6128,14 +6128,14 @@
       <c r="R1" s="24"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -6258,7 +6258,7 @@
         <v>677</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G5" s="44" t="s">
         <v>67</v>
@@ -6271,6 +6271,13 @@
       </c>
       <c r="L5" s="44">
         <v>19</v>
+      </c>
+      <c r="M5" s="44">
+        <v>18</v>
+      </c>
+      <c r="N5" s="44">
+        <f>(L5-K5)/6</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="R5" s="44" t="s">
         <v>663</v>
@@ -6292,6 +6299,7 @@
       <c r="E6" s="42" t="s">
         <v>71</v>
       </c>
+      <c r="N6" s="44"/>
     </row>
     <row r="7" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="42" t="s">
@@ -6304,7 +6312,7 @@
         <v>193</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G7" s="42" t="s">
         <v>67</v>
@@ -6318,6 +6326,13 @@
       <c r="L7" s="42">
         <v>4</v>
       </c>
+      <c r="M7" s="42">
+        <v>2</v>
+      </c>
+      <c r="N7" s="44">
+        <f t="shared" ref="N6:N15" si="0">(L7-K7)/6</f>
+        <v>0.66666666666666663</v>
+      </c>
       <c r="R7" s="42" t="s">
         <v>663</v>
       </c>
@@ -6341,6 +6356,7 @@
       <c r="I8" s="42">
         <v>0</v>
       </c>
+      <c r="N8" s="44"/>
     </row>
     <row r="9" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="42" t="s">
@@ -6361,6 +6377,7 @@
       <c r="I9" s="42" t="b">
         <v>1</v>
       </c>
+      <c r="N9" s="44"/>
     </row>
     <row r="10" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="42" t="b">
@@ -6378,6 +6395,7 @@
       <c r="E10" s="42" t="s">
         <v>71</v>
       </c>
+      <c r="N10" s="44"/>
     </row>
     <row r="11" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="42" t="s">
@@ -6401,6 +6419,7 @@
       <c r="J11" s="42" t="s">
         <v>86</v>
       </c>
+      <c r="N11" s="44"/>
     </row>
     <row r="12" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="42" t="s">
@@ -6413,7 +6432,7 @@
         <v>291</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>67</v>
@@ -6426,6 +6445,13 @@
       </c>
       <c r="L12" s="42">
         <v>10</v>
+      </c>
+      <c r="M12" s="42">
+        <v>5</v>
+      </c>
+      <c r="N12" s="44">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="R12" s="42" t="s">
         <v>663</v>
@@ -6447,6 +6473,7 @@
       <c r="E13" s="42" t="s">
         <v>71</v>
       </c>
+      <c r="N13" s="44"/>
     </row>
     <row r="14" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="42" t="s">
@@ -6470,6 +6497,7 @@
       <c r="J14" s="42" t="s">
         <v>86</v>
       </c>
+      <c r="N14" s="44"/>
     </row>
     <row r="15" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="42" t="s">
@@ -6482,7 +6510,7 @@
         <v>49</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>67</v>
@@ -6495,6 +6523,13 @@
       </c>
       <c r="L15" s="42">
         <v>10</v>
+      </c>
+      <c r="M15" s="42">
+        <v>5</v>
+      </c>
+      <c r="N15" s="44">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="R15" s="42" t="s">
         <v>663</v>
@@ -6537,29 +6572,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="b">
+    <row r="18" spans="1:26" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>691</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="45" t="s">
         <v>690</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="45" t="s">
         <v>690</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
     </row>
     <row r="19" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>

</xml_diff>

<commit_message>
Updating audit 662 project
</commit_message>
<xml_diff>
--- a/projects/audit662.xlsx
+++ b/projects/audit662.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="60" windowWidth="2964" windowHeight="9048" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="16800" yWindow="60" windowWidth="2964" windowHeight="9048" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Lookups" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$G$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$G$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$7</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="683">
   <si>
     <t>type</t>
   </si>
@@ -1474,9 +1474,6 @@
     <t>Outputs</t>
   </si>
   <si>
-    <t>MJ/m2</t>
-  </si>
-  <si>
     <t>OpenStudio Server Version</t>
   </si>
   <si>
@@ -1690,15 +1687,6 @@
     <t>Set Hot Water Loop Temperature</t>
   </si>
   <si>
-    <t>total_natural_gas</t>
-  </si>
-  <si>
-    <t>Total Electricity</t>
-  </si>
-  <si>
-    <t>total_electricity</t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
@@ -1864,9 +1852,6 @@
     <t>positive integer (if individual, total simulations is this times each variable)</t>
   </si>
   <si>
-    <t>Total Natural Gas</t>
-  </si>
-  <si>
     <t>m3.large</t>
   </si>
   <si>
@@ -1954,9 +1939,6 @@
     <t xml:space="preserve"> - Worker Only - </t>
   </si>
   <si>
-    <t>Office Sampling</t>
-  </si>
-  <si>
     <t>cooling_electricity_jan</t>
   </si>
   <si>
@@ -2035,18 +2017,6 @@
     <t>uniform_uncertain</t>
   </si>
   <si>
-    <t>Heating Natural Gas</t>
-  </si>
-  <si>
-    <t>heating_natural_gas</t>
-  </si>
-  <si>
-    <t>Cooling Electricity</t>
-  </si>
-  <si>
-    <t>cooling_electricity</t>
-  </si>
-  <si>
     <t>0.2.3</t>
   </si>
   <si>
@@ -2117,6 +2087,9 @@
   </si>
   <si>
     <t>Calibration Reports</t>
+  </si>
+  <si>
+    <t>Audit 662</t>
   </si>
 </sst>
 </file>
@@ -3695,7 +3668,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3765,7 +3738,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5545,8 +5517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5582,7 +5554,7 @@
         <v>439</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>440</v>
@@ -5593,7 +5565,7 @@
         <v>461</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>462</v>
@@ -5601,24 +5573,24 @@
     </row>
     <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="46.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -5626,18 +5598,18 @@
         <v>445</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>608</v>
-      </c>
-      <c r="C7" s="38" t="str">
+        <v>603</v>
+      </c>
+      <c r="C7" s="37" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
         <v>2 Cores - Recommended for Server</v>
       </c>
-      <c r="D7" s="38" t="str">
+      <c r="D7" s="37" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
         <v>$0.14/hour</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -5647,11 +5619,11 @@
       <c r="B8" s="28" t="s">
         <v>443</v>
       </c>
-      <c r="C8" s="38" t="str">
+      <c r="C8" s="37" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
         <v>8 Cores - Worker Only - Recommended for Worker</v>
       </c>
-      <c r="D8" s="38" t="str">
+      <c r="D8" s="37" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
         <v>$0.42/hour</v>
       </c>
@@ -5667,9 +5639,9 @@
         <v>0</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="38"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="2" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -5686,10 +5658,10 @@
         <v>41</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>637</v>
+        <v>682</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -5697,10 +5669,10 @@
         <v>26</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -5730,7 +5702,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -5749,7 +5721,7 @@
         <v>475</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>440</v>
@@ -5760,7 +5732,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -5785,13 +5757,13 @@
         <v>454</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>460</v>
@@ -5806,11 +5778,11 @@
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v>all_variables</v>
       </c>
-      <c r="C24" s="39" t="str">
+      <c r="C24" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v>individual_variables / all_variables</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="39" t="s">
         <v>457</v>
       </c>
     </row>
@@ -5820,14 +5792,14 @@
         <v>Number of Samples</v>
       </c>
       <c r="B25" s="29">
-        <v>30</v>
-      </c>
-      <c r="C25" s="39" t="str">
+        <v>300</v>
+      </c>
+      <c r="C25" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
-      <c r="D25" s="40">
-        <v>2</v>
+      <c r="D25" s="39">
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -5839,11 +5811,11 @@
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C26" s="39" t="str">
+      <c r="C26" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D26" s="40"/>
+      <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="str">
@@ -5854,11 +5826,11 @@
         <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C27" s="39" t="str">
+      <c r="C27" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D27" s="40"/>
+      <c r="D27" s="39"/>
     </row>
     <row r="28" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="str">
@@ -5869,11 +5841,11 @@
         <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C28" s="39" t="str">
+      <c r="C28" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D28" s="40"/>
+      <c r="D28" s="39"/>
     </row>
     <row r="29" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="str">
@@ -5884,11 +5856,11 @@
         <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C29" s="39" t="str">
+      <c r="C29" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D29" s="40"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="str">
@@ -5899,11 +5871,11 @@
         <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C30" s="39" t="str">
+      <c r="C30" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D30" s="40"/>
+      <c r="D30" s="39"/>
     </row>
     <row r="31" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="str">
@@ -5914,11 +5886,11 @@
         <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C31" s="39" t="str">
+      <c r="C31" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D31" s="40"/>
+      <c r="D31" s="39"/>
     </row>
     <row r="32" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34" t="str">
@@ -5929,11 +5901,11 @@
         <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C32" s="39" t="str">
+      <c r="C32" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D32" s="40"/>
+      <c r="D32" s="39"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="34" t="str">
@@ -5944,11 +5916,11 @@
         <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C33" s="39" t="str">
+      <c r="C33" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D33" s="40"/>
+      <c r="D33" s="39"/>
     </row>
     <row r="34" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="34" t="str">
@@ -5959,11 +5931,11 @@
         <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C34" s="39" t="str">
+      <c r="C34" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D34" s="40"/>
+      <c r="D34" s="39"/>
     </row>
     <row r="35" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="29"/>
@@ -5987,8 +5959,8 @@
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="41" t="s">
-        <v>671</v>
+      <c r="B37" s="40" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6013,13 +5985,13 @@
         <v>33</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="40" t="s">
-        <v>673</v>
+      <c r="D40" s="39" t="s">
+        <v>663</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>453</v>
@@ -6033,11 +6005,11 @@
         <v>35</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>
@@ -6072,8 +6044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6090,7 +6062,7 @@
     <col min="10" max="10" width="8.6640625" style="4" customWidth="1"/>
     <col min="11" max="11" width="7.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="7.6640625" style="1" customWidth="1"/>
     <col min="16" max="17" width="11.44140625" style="1"/>
     <col min="18" max="18" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -6115,27 +6087,27 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
-      <c r="P1" s="36" t="s">
-        <v>484</v>
+      <c r="P1" s="35" t="s">
+        <v>483</v>
       </c>
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -6145,10 +6117,10 @@
         <v>38</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -6197,13 +6169,13 @@
         <v>9</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="P3" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q3" s="16" t="s">
         <v>485</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>486</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>8</v>
@@ -6230,371 +6202,378 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="b">
+    <row r="4" spans="1:26" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="44" t="s">
-        <v>675</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>674</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>674</v>
-      </c>
-      <c r="E4" s="44" t="s">
+      <c r="B4" s="43" t="s">
+        <v>665</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>664</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>664</v>
+      </c>
+      <c r="E4" s="43" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="44" t="s">
+    <row r="5" spans="1:26" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>676</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>677</v>
-      </c>
-      <c r="F5" s="44" t="s">
+      <c r="D5" s="43" t="s">
+        <v>666</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>667</v>
+      </c>
+      <c r="F5" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="43">
         <v>18.899999999999999</v>
       </c>
-      <c r="K5" s="44">
+      <c r="K5" s="43">
         <v>17</v>
       </c>
-      <c r="L5" s="44">
+      <c r="L5" s="43">
         <v>19</v>
       </c>
-      <c r="M5" s="44">
+      <c r="M5" s="43">
         <v>18</v>
       </c>
-      <c r="N5" s="44">
+      <c r="N5" s="43">
         <f>(L5-K5)/6</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="R5" s="44" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="b">
+      <c r="R5" s="43" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>678</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>678</v>
-      </c>
-      <c r="E6" s="42" t="s">
+      <c r="C6" s="41" t="s">
+        <v>668</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="N6" s="44"/>
-    </row>
-    <row r="7" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="42" t="s">
+    </row>
+    <row r="7" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="41" t="s">
+        <v>669</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="41">
+        <v>0</v>
+      </c>
+      <c r="K7" s="41">
+        <v>0</v>
+      </c>
+      <c r="L7" s="41">
+        <v>4</v>
+      </c>
+      <c r="M7" s="41">
+        <v>2</v>
+      </c>
+      <c r="N7" s="41">
+        <f t="shared" ref="N7:N15" si="0">(L7-K7)/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R7" s="41" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="41" t="s">
         <v>679</v>
       </c>
-      <c r="E7" s="42" t="s">
-        <v>193</v>
-      </c>
-      <c r="F7" s="42" t="s">
+      <c r="E8" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>670</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>671</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>376</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>672</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="F12" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G12" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="42">
-        <v>0</v>
-      </c>
-      <c r="K7" s="42">
-        <v>0</v>
-      </c>
-      <c r="L7" s="42">
-        <v>4</v>
-      </c>
-      <c r="M7" s="42">
-        <v>2</v>
-      </c>
-      <c r="N7" s="44">
-        <f t="shared" ref="N6:N15" si="0">(L7-K7)/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="R7" s="42" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>689</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="42">
-        <v>0</v>
-      </c>
-      <c r="N8" s="44"/>
-    </row>
-    <row r="9" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>680</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="I9" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" s="44"/>
-    </row>
-    <row r="10" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>288</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>681</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>681</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="N10" s="44"/>
-    </row>
-    <row r="11" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>376</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="N11" s="44"/>
-    </row>
-    <row r="12" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>682</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>291</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="42">
-        <v>0</v>
-      </c>
-      <c r="K12" s="42">
-        <v>0</v>
-      </c>
-      <c r="L12" s="42">
+      <c r="I12" s="41">
+        <v>0</v>
+      </c>
+      <c r="K12" s="41">
+        <v>0</v>
+      </c>
+      <c r="L12" s="41">
         <v>10</v>
       </c>
-      <c r="M12" s="42">
+      <c r="M12" s="41">
         <v>5</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="41">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="R12" s="42" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="b">
+      <c r="R12" s="41" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="42" t="s">
-        <v>683</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>683</v>
-      </c>
-      <c r="E13" s="42" t="s">
+      <c r="C13" s="41" t="s">
+        <v>673</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="44"/>
-    </row>
-    <row r="14" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="42" t="s">
+    </row>
+    <row r="14" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="42" t="s">
+      <c r="F14" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="J14" s="42" t="s">
+      <c r="J14" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="N14" s="44"/>
-    </row>
-    <row r="15" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="42" t="s">
+    </row>
+    <row r="15" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>684</v>
-      </c>
-      <c r="E15" s="42" t="s">
+      <c r="D15" s="41" t="s">
+        <v>674</v>
+      </c>
+      <c r="E15" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="42">
-        <v>0</v>
-      </c>
-      <c r="K15" s="42">
-        <v>0</v>
-      </c>
-      <c r="L15" s="42">
+      <c r="I15" s="41">
+        <v>0</v>
+      </c>
+      <c r="K15" s="41">
+        <v>0</v>
+      </c>
+      <c r="L15" s="41">
         <v>10</v>
       </c>
-      <c r="M15" s="42">
+      <c r="M15" s="41">
         <v>5</v>
       </c>
-      <c r="N15" s="44">
-        <f t="shared" si="0"/>
+      <c r="N15" s="41">
+        <f>(L15-K15)/6</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="R15" s="42" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="b">
+      <c r="R15" s="41" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="43" t="s">
-        <v>686</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>685</v>
-      </c>
-      <c r="D16" s="43" t="s">
-        <v>685</v>
-      </c>
-      <c r="E16" s="43" t="s">
+      <c r="B16" s="42" t="s">
+        <v>676</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>675</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>675</v>
+      </c>
+      <c r="E16" s="42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>688</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>687</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="43" t="s">
+    <row r="17" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>678</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>677</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="b">
+      <c r="I17" s="42">
+        <v>2</v>
+      </c>
+      <c r="K17" s="42">
+        <v>2</v>
+      </c>
+      <c r="L17" s="42">
+        <v>3.5</v>
+      </c>
+      <c r="M17" s="42">
+        <f>AVERAGE(K17:L17)</f>
+        <v>2.75</v>
+      </c>
+      <c r="N17" s="42">
+        <f>(L17-K17)/6</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" s="45" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="45" t="s">
-        <v>691</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>690</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>690</v>
-      </c>
-      <c r="E18" s="45" t="s">
+      <c r="B18" s="44" t="s">
+        <v>681</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>680</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>680</v>
+      </c>
+      <c r="E18" s="44" t="s">
         <v>236</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
@@ -7293,11 +7272,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7312,7 +7291,7 @@
     <col min="8" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="7" t="s">
@@ -7323,7 +7302,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>464</v>
       </c>
@@ -7340,13 +7319,13 @@
         <v>468</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
@@ -7357,477 +7336,431 @@
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="10" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>607</v>
+        <v>632</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>549</v>
+        <v>632</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>477</v>
+        <v>633</v>
       </c>
       <c r="D4" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="33"/>
+      <c r="E4" s="36">
+        <v>201214800000</v>
+      </c>
+      <c r="F4" s="32"/>
       <c r="G4" s="33"/>
     </row>
-    <row r="5" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>550</v>
+        <v>634</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>551</v>
+        <v>634</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>477</v>
+        <v>633</v>
       </c>
       <c r="D5" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="33"/>
+      <c r="E5" s="36">
+        <v>208771200000</v>
+      </c>
+      <c r="F5" s="32"/>
       <c r="G5" s="33"/>
     </row>
-    <row r="6" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>664</v>
+        <v>635</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>665</v>
+        <v>635</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>477</v>
+        <v>633</v>
       </c>
       <c r="D6" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="36">
+        <v>195645600000</v>
+      </c>
+      <c r="F6" s="32"/>
       <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>666</v>
+        <v>636</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>667</v>
+        <v>636</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>477</v>
+        <v>633</v>
       </c>
       <c r="D7" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="E7" s="36">
+        <v>183265200000</v>
+      </c>
+      <c r="F7" s="32"/>
       <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D8" s="33" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E8" s="36">
+        <v>162770400000</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
     </row>
-    <row r="9" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D9" s="33" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E9" s="36">
+        <v>193197600000</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="33"/>
     </row>
-    <row r="10" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D10" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="36">
+        <v>181231200000</v>
+      </c>
       <c r="F10" s="32"/>
       <c r="G10" s="33"/>
     </row>
-    <row r="11" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D11" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="36">
+        <v>189968400000</v>
+      </c>
       <c r="F11" s="32"/>
       <c r="G11" s="33"/>
     </row>
-    <row r="12" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D12" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="36">
+        <v>157928400000</v>
+      </c>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
     </row>
-    <row r="13" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
+        <v>642</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>642</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D13" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="36">
+        <v>181404000000</v>
+      </c>
+      <c r="F13" s="32"/>
+    </row>
+    <row r="14" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>643</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>643</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D14" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="36">
+        <v>187452000000</v>
+      </c>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
         <v>644</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B15" s="33" t="s">
         <v>644</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D13" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+      <c r="C15" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D15" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="32">
+        <v>207900000000</v>
+      </c>
+      <c r="F15" s="32"/>
+    </row>
+    <row r="16" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
         <v>645</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B16" s="33" t="s">
         <v>645</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D14" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>646</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>646</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D15" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>647</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>647</v>
-      </c>
       <c r="C16" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D16" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="E16" s="37"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D17" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
+        <v>647</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>647</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D18" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="36"/>
+      <c r="F18" s="32"/>
+    </row>
+    <row r="19" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D19" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33" t="s">
         <v>649</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B20" s="33" t="s">
         <v>649</v>
       </c>
-      <c r="C18" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D18" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="32"/>
-    </row>
-    <row r="19" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="C20" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D20" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B21" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="C19" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D19" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-    </row>
-    <row r="20" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="C21" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="D21" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>651</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B22" s="33" t="s">
         <v>651</v>
       </c>
-      <c r="C20" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D20" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="32"/>
-    </row>
-    <row r="21" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D21" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="32"/>
-    </row>
-    <row r="22" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>653</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>653</v>
-      </c>
       <c r="C22" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D22" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="E22" s="37"/>
       <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D23" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="E23" s="37"/>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D24" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="E24" s="37"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D25" s="33" t="b">
         <v>0</v>
       </c>
+      <c r="E25" s="36"/>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D26" s="33" t="b">
         <v>0</v>
       </c>
+      <c r="E26" s="36"/>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D27" s="33" t="b">
         <v>0</v>
       </c>
+      <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="33"/>
-    </row>
-    <row r="28" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
-        <v>659</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>659</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D28" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="33" t="s">
-        <v>660</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>660</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D29" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-    </row>
-    <row r="30" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
-        <v>661</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>661</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D30" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
-    </row>
-    <row r="31" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
-        <v>662</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>662</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="D31" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15200,10 +15133,10 @@
         <v>0</v>
       </c>
       <c r="B328" t="s">
+        <v>486</v>
+      </c>
+      <c r="C328" t="s">
         <v>487</v>
-      </c>
-      <c r="C328" t="s">
-        <v>488</v>
       </c>
       <c r="D328" t="s">
         <v>71</v>
@@ -15214,10 +15147,10 @@
         <v>22</v>
       </c>
       <c r="C329" t="s">
+        <v>488</v>
+      </c>
+      <c r="D329" t="s">
         <v>489</v>
-      </c>
-      <c r="D329" t="s">
-        <v>490</v>
       </c>
       <c r="E329" t="s">
         <v>2</v>
@@ -15226,10 +15159,10 @@
         <v>65</v>
       </c>
       <c r="H329" t="s">
+        <v>490</v>
+      </c>
+      <c r="I329" t="s">
         <v>491</v>
-      </c>
-      <c r="I329" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -15237,10 +15170,10 @@
         <v>22</v>
       </c>
       <c r="C330" t="s">
+        <v>492</v>
+      </c>
+      <c r="D330" t="s">
         <v>493</v>
-      </c>
-      <c r="D330" t="s">
-        <v>494</v>
       </c>
       <c r="E330" t="s">
         <v>2</v>
@@ -15257,10 +15190,10 @@
         <v>22</v>
       </c>
       <c r="C331" t="s">
+        <v>494</v>
+      </c>
+      <c r="D331" t="s">
         <v>495</v>
-      </c>
-      <c r="D331" t="s">
-        <v>496</v>
       </c>
       <c r="E331" t="s">
         <v>2</v>
@@ -15277,10 +15210,10 @@
         <v>22</v>
       </c>
       <c r="C332" t="s">
+        <v>496</v>
+      </c>
+      <c r="D332" t="s">
         <v>497</v>
-      </c>
-      <c r="D332" t="s">
-        <v>498</v>
       </c>
       <c r="E332" t="s">
         <v>2</v>
@@ -15297,10 +15230,10 @@
         <v>22</v>
       </c>
       <c r="C333" t="s">
+        <v>498</v>
+      </c>
+      <c r="D333" t="s">
         <v>499</v>
-      </c>
-      <c r="D333" t="s">
-        <v>500</v>
       </c>
       <c r="E333" t="s">
         <v>2</v>
@@ -15314,10 +15247,10 @@
         <v>22</v>
       </c>
       <c r="C334" t="s">
+        <v>500</v>
+      </c>
+      <c r="D334" t="s">
         <v>501</v>
-      </c>
-      <c r="D334" t="s">
-        <v>502</v>
       </c>
       <c r="E334" t="s">
         <v>2</v>
@@ -15326,10 +15259,10 @@
         <v>65</v>
       </c>
       <c r="H334" t="s">
+        <v>502</v>
+      </c>
+      <c r="I334" t="s">
         <v>503</v>
-      </c>
-      <c r="I334" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -15337,10 +15270,10 @@
         <v>22</v>
       </c>
       <c r="C335" t="s">
+        <v>504</v>
+      </c>
+      <c r="D335" t="s">
         <v>505</v>
-      </c>
-      <c r="D335" t="s">
-        <v>506</v>
       </c>
       <c r="E335" t="s">
         <v>2</v>
@@ -15349,10 +15282,10 @@
         <v>65</v>
       </c>
       <c r="H335" t="s">
+        <v>506</v>
+      </c>
+      <c r="I335" t="s">
         <v>507</v>
-      </c>
-      <c r="I335" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -15360,10 +15293,10 @@
         <v>0</v>
       </c>
       <c r="B336" t="s">
+        <v>508</v>
+      </c>
+      <c r="C336" t="s">
         <v>509</v>
-      </c>
-      <c r="C336" t="s">
-        <v>510</v>
       </c>
       <c r="D336" t="s">
         <v>71</v>
@@ -15374,10 +15307,10 @@
         <v>22</v>
       </c>
       <c r="C337" t="s">
+        <v>510</v>
+      </c>
+      <c r="D337" t="s">
         <v>511</v>
-      </c>
-      <c r="D337" t="s">
-        <v>512</v>
       </c>
       <c r="E337" t="s">
         <v>2</v>
@@ -15386,10 +15319,10 @@
         <v>65</v>
       </c>
       <c r="H337" t="s">
+        <v>512</v>
+      </c>
+      <c r="I337" t="s">
         <v>513</v>
-      </c>
-      <c r="I337" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="338" spans="1:16" x14ac:dyDescent="0.3">
@@ -15397,10 +15330,10 @@
         <v>22</v>
       </c>
       <c r="C338" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D338" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E338" t="s">
         <v>2</v>
@@ -15409,10 +15342,10 @@
         <v>65</v>
       </c>
       <c r="H338" t="s">
+        <v>515</v>
+      </c>
+      <c r="I338" t="s">
         <v>516</v>
-      </c>
-      <c r="I338" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="339" spans="1:16" x14ac:dyDescent="0.3">
@@ -15420,10 +15353,10 @@
         <v>22</v>
       </c>
       <c r="C339" t="s">
+        <v>517</v>
+      </c>
+      <c r="D339" t="s">
         <v>518</v>
-      </c>
-      <c r="D339" t="s">
-        <v>519</v>
       </c>
       <c r="E339" t="s">
         <v>2</v>
@@ -15440,10 +15373,10 @@
         <v>22</v>
       </c>
       <c r="C340" t="s">
+        <v>519</v>
+      </c>
+      <c r="D340" t="s">
         <v>520</v>
-      </c>
-      <c r="D340" t="s">
-        <v>521</v>
       </c>
       <c r="E340" t="s">
         <v>2</v>
@@ -15460,10 +15393,10 @@
         <v>22</v>
       </c>
       <c r="C341" t="s">
+        <v>521</v>
+      </c>
+      <c r="D341" t="s">
         <v>522</v>
-      </c>
-      <c r="D341" t="s">
-        <v>523</v>
       </c>
       <c r="E341" t="s">
         <v>2</v>
@@ -15477,10 +15410,10 @@
         <v>0</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D342" s="1" t="s">
         <v>71</v>
@@ -15504,10 +15437,10 @@
         <v>22</v>
       </c>
       <c r="C343" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D343" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E343" t="s">
         <v>2</v>
@@ -15516,10 +15449,10 @@
         <v>65</v>
       </c>
       <c r="H343" t="s">
+        <v>528</v>
+      </c>
+      <c r="I343" t="s">
         <v>529</v>
-      </c>
-      <c r="I343" t="s">
-        <v>530</v>
       </c>
       <c r="L343" s="1"/>
       <c r="M343" s="1"/>
@@ -15533,10 +15466,10 @@
         <v>22</v>
       </c>
       <c r="C344" t="s">
+        <v>526</v>
+      </c>
+      <c r="D344" t="s">
         <v>527</v>
-      </c>
-      <c r="D344" t="s">
-        <v>528</v>
       </c>
       <c r="E344" t="s">
         <v>2</v>
@@ -15571,10 +15504,10 @@
         <v>0</v>
       </c>
       <c r="B345" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C345" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D345" s="1" t="s">
         <v>71</v>
@@ -15585,10 +15518,10 @@
         <v>22</v>
       </c>
       <c r="C346" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E346" t="s">
         <v>2</v>
@@ -15799,10 +15732,10 @@
         <v>0</v>
       </c>
       <c r="B357" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C357" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D357" t="s">
         <v>71</v>
@@ -15813,10 +15746,10 @@
         <v>22</v>
       </c>
       <c r="C358" t="s">
+        <v>536</v>
+      </c>
+      <c r="D358" t="s">
         <v>537</v>
-      </c>
-      <c r="D358" t="s">
-        <v>538</v>
       </c>
       <c r="E358" t="s">
         <v>2</v>
@@ -15833,10 +15766,10 @@
         <v>22</v>
       </c>
       <c r="C359" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D359" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E359" t="s">
         <v>2</v>
@@ -15853,10 +15786,10 @@
         <v>0</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D360" s="1" t="s">
         <v>71</v>
@@ -15869,10 +15802,10 @@
         <v>22</v>
       </c>
       <c r="C361" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D361" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E361" t="s">
         <v>2</v>
@@ -15882,10 +15815,10 @@
       </c>
       <c r="G361"/>
       <c r="H361" t="s">
+        <v>528</v>
+      </c>
+      <c r="I361" t="s">
         <v>529</v>
-      </c>
-      <c r="I361" t="s">
-        <v>530</v>
       </c>
       <c r="J361"/>
       <c r="K361"/>
@@ -15896,10 +15829,10 @@
         <v>23</v>
       </c>
       <c r="C362" t="s">
+        <v>526</v>
+      </c>
+      <c r="D362" t="s">
         <v>527</v>
-      </c>
-      <c r="D362" t="s">
-        <v>528</v>
       </c>
       <c r="E362" t="s">
         <v>15</v>
@@ -15936,10 +15869,10 @@
         <v>0</v>
       </c>
       <c r="B363" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C363" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>71</v>
@@ -15950,10 +15883,10 @@
         <v>22</v>
       </c>
       <c r="C364" t="s">
+        <v>542</v>
+      </c>
+      <c r="D364" t="s">
         <v>543</v>
-      </c>
-      <c r="D364" t="s">
-        <v>544</v>
       </c>
       <c r="E364" t="s">
         <v>2</v>
@@ -15970,10 +15903,10 @@
         <v>0</v>
       </c>
       <c r="B365" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C365" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D365" s="1" t="s">
         <v>71</v>
@@ -15984,10 +15917,10 @@
         <v>22</v>
       </c>
       <c r="C366" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D366" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E366" t="s">
         <v>2</v>
@@ -16041,72 +15974,72 @@
     </row>
     <row r="2" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>448</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>449</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>450</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>448</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>449</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -16117,52 +16050,52 @@
         <v>450</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>450</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>451</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="E11" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="G11" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -16173,7 +16106,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G12" t="s">
         <v>474</v>
@@ -16187,66 +16120,66 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="33" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C16" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="L16" t="s">
+        <v>573</v>
+      </c>
+      <c r="O16" t="s">
         <v>577</v>
       </c>
-      <c r="O16" t="s">
-        <v>581</v>
-      </c>
       <c r="R16" s="33" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="U16" s="33" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="F17" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="G17" t="s">
         <v>459</v>
       </c>
       <c r="H17" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J17" s="32">
         <v>0.01</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="M17">
         <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="O17" t="s">
         <v>4</v>
@@ -16255,7 +16188,7 @@
         <v>30</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -16269,229 +16202,229 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="J18" s="32">
         <v>0.01</v>
       </c>
       <c r="K18" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="L18" s="34" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="M18">
         <v>5</v>
       </c>
       <c r="N18" s="33" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="O18" s="34" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="P18">
         <v>3</v>
       </c>
       <c r="Q18" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J19" s="32">
         <v>45036000000000</v>
       </c>
       <c r="K19" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="M19">
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="P19">
         <v>0.85</v>
       </c>
       <c r="Q19" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="L20" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="M20">
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="O20" s="34" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="P20">
         <v>2</v>
       </c>
       <c r="Q20" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="M21" s="32">
         <v>0.01</v>
       </c>
       <c r="N21" s="34" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="O21" s="34" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="P21">
         <v>2</v>
       </c>
       <c r="Q21" s="33" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="J22" s="34">
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="M22" s="32">
         <v>0.01</v>
       </c>
       <c r="N22" s="34" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="O22" s="34" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="P22">
         <v>0.8</v>
       </c>
       <c r="Q22" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="M23" s="32">
         <v>0.01</v>
       </c>
       <c r="N23" s="33" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="O23" s="34" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="P23" s="34" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L24" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="M24" s="32">
         <v>45036000000000</v>
       </c>
       <c r="N24" s="33" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="O24" s="34" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="P24" s="34">
         <v>2</v>
       </c>
       <c r="Q24" s="33" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L25" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="M25" s="33">
         <v>100</v>
       </c>
       <c r="N25" s="33" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L26" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L27" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="M27" s="34">
         <v>2</v>
       </c>
       <c r="N27" s="33" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating to new objective function
</commit_message>
<xml_diff>
--- a/projects/audit662.xlsx
+++ b/projects/audit662.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7932" yWindow="-120" windowWidth="14040" windowHeight="9048" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="7932" yWindow="-120" windowWidth="14040" windowHeight="9048" tabRatio="562" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="671">
   <si>
     <t>type</t>
   </si>
@@ -1942,81 +1942,9 @@
     <t xml:space="preserve"> - Worker Only - </t>
   </si>
   <si>
-    <t>cooling_electricity_jan</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
-    <t>cooling_electricity_feb</t>
-  </si>
-  <si>
-    <t>cooling_electricity_mar</t>
-  </si>
-  <si>
-    <t>cooling_electricity_apr</t>
-  </si>
-  <si>
-    <t>cooling_electricity_may</t>
-  </si>
-  <si>
-    <t>cooling_electricity_jun</t>
-  </si>
-  <si>
-    <t>cooling_electricity_jul</t>
-  </si>
-  <si>
-    <t>cooling_electricity_aug</t>
-  </si>
-  <si>
-    <t>cooling_electricity_sep</t>
-  </si>
-  <si>
-    <t>cooling_electricity_oct</t>
-  </si>
-  <si>
-    <t>cooling_electricity_nov</t>
-  </si>
-  <si>
-    <t>cooling_electricity_dec</t>
-  </si>
-  <si>
-    <t>heating_gas_jan</t>
-  </si>
-  <si>
-    <t>heating_gas_feb</t>
-  </si>
-  <si>
-    <t>heating_gas_mar</t>
-  </si>
-  <si>
-    <t>heating_gas_apr</t>
-  </si>
-  <si>
-    <t>heating_gas_may</t>
-  </si>
-  <si>
-    <t>heating_gas_jun</t>
-  </si>
-  <si>
-    <t>heating_gas_jul</t>
-  </si>
-  <si>
-    <t>heating_gas_aug</t>
-  </si>
-  <si>
-    <t>heating_gas_sep</t>
-  </si>
-  <si>
-    <t>heating_gas_oct</t>
-  </si>
-  <si>
-    <t>heating_gas_nov</t>
-  </si>
-  <si>
-    <t>heating_gas_dec</t>
-  </si>
-  <si>
     <t>uniform_uncertain</t>
   </si>
   <si>
@@ -2093,6 +2021,42 @@
   </si>
   <si>
     <t>Audit 662 Optimization</t>
+  </si>
+  <si>
+    <t>total_electricity_nov</t>
+  </si>
+  <si>
+    <t>total_electricity_jan</t>
+  </si>
+  <si>
+    <t>total_electricity_feb</t>
+  </si>
+  <si>
+    <t>total_electricity_mar</t>
+  </si>
+  <si>
+    <t>total_electricity_apr</t>
+  </si>
+  <si>
+    <t>total_electricity_may</t>
+  </si>
+  <si>
+    <t>total_electricity_jun</t>
+  </si>
+  <si>
+    <t>total_electricity_jul</t>
+  </si>
+  <si>
+    <t>total_electricity_aug</t>
+  </si>
+  <si>
+    <t>total_electricity_sep</t>
+  </si>
+  <si>
+    <t>total_electricity_oct</t>
+  </si>
+  <si>
+    <t>total_electricity_dec</t>
   </si>
 </sst>
 </file>
@@ -5816,8 +5780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5853,7 +5817,7 @@
         <v>439</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>658</v>
+        <v>634</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>440</v>
@@ -5875,7 +5839,7 @@
         <v>477</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>659</v>
+        <v>635</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>630</v>
@@ -5957,7 +5921,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>682</v>
+        <v>658</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>479</v>
@@ -5968,7 +5932,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>660</v>
+        <v>636</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>481</v>
@@ -6075,15 +6039,15 @@
       </c>
       <c r="B24" s="29">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX([1]Lookups!$C$17:$Z$26,1,3*MATCH([1]Setup!$B21,[1]Lookups!$A$17:$A$23,0)-1))=0,"",INDEX([1]Lookups!$C$17:$Z$26,1,3*MATCH([1]Setup!$B21,[1]Lookups!$A$17:$A$23,0)-1)))</f>
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C24" s="38" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v>Size of initial population</v>
       </c>
       <c r="D24" s="39">
-        <f>(11+12+12)*2</f>
-        <v>70</v>
+        <f>(11+12)*2</f>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -6261,7 +6225,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>661</v>
+        <v>637</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6286,13 +6250,13 @@
         <v>33</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>662</v>
+        <v>638</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>663</v>
+        <v>639</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>453</v>
@@ -6508,13 +6472,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>665</v>
+        <v>641</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>664</v>
+        <v>640</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>664</v>
+        <v>640</v>
       </c>
       <c r="E4" s="43" t="s">
         <v>71</v>
@@ -6525,10 +6489,10 @@
         <v>23</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>666</v>
+        <v>642</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>667</v>
+        <v>643</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>15</v>
@@ -6553,7 +6517,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="R5" s="43" t="s">
-        <v>657</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
@@ -6564,7 +6528,7 @@
         <v>190</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>668</v>
+        <v>644</v>
       </c>
       <c r="D6" s="41" t="s">
         <v>191</v>
@@ -6578,7 +6542,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>669</v>
+        <v>645</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>193</v>
@@ -6606,7 +6570,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="R7" s="41" t="s">
-        <v>657</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
@@ -6614,7 +6578,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>679</v>
+        <v>655</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>195</v>
@@ -6634,7 +6598,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>670</v>
+        <v>646</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>197</v>
@@ -6657,7 +6621,7 @@
         <v>288</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>671</v>
+        <v>647</v>
       </c>
       <c r="D10" s="41" t="s">
         <v>289</v>
@@ -6694,7 +6658,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>672</v>
+        <v>648</v>
       </c>
       <c r="E12" s="41" t="s">
         <v>291</v>
@@ -6722,7 +6686,7 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="R12" s="41" t="s">
-        <v>657</v>
+        <v>633</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
@@ -6733,7 +6697,7 @@
         <v>70</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>673</v>
+        <v>649</v>
       </c>
       <c r="D13" s="41" t="s">
         <v>46</v>
@@ -6770,7 +6734,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>674</v>
+        <v>650</v>
       </c>
       <c r="E15" s="41" t="s">
         <v>49</v>
@@ -6798,7 +6762,7 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="R15" s="41" t="s">
-        <v>657</v>
+        <v>633</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.3">
@@ -6806,13 +6770,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>676</v>
+        <v>652</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>675</v>
+        <v>651</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>675</v>
+        <v>651</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>71</v>
@@ -6823,10 +6787,10 @@
         <v>22</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>678</v>
+        <v>654</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>677</v>
+        <v>653</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>2</v>
@@ -6857,13 +6821,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>681</v>
+        <v>657</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>680</v>
+        <v>656</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>680</v>
+        <v>656</v>
       </c>
       <c r="E18" s="44" t="s">
         <v>236</v>
@@ -7573,11 +7537,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7642,13 +7606,13 @@
     </row>
     <row r="4" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
+        <v>660</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>660</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>632</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>632</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>633</v>
       </c>
       <c r="D4" s="33" t="b">
         <v>1</v>
@@ -7661,13 +7625,13 @@
     </row>
     <row r="5" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>634</v>
+        <v>661</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>634</v>
+        <v>661</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D5" s="33" t="b">
         <v>1</v>
@@ -7680,13 +7644,13 @@
     </row>
     <row r="6" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>635</v>
+        <v>662</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>635</v>
+        <v>662</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D6" s="33" t="b">
         <v>1</v>
@@ -7699,13 +7663,13 @@
     </row>
     <row r="7" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>636</v>
+        <v>663</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>636</v>
+        <v>663</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D7" s="33" t="b">
         <v>1</v>
@@ -7718,13 +7682,13 @@
     </row>
     <row r="8" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>637</v>
+        <v>664</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>637</v>
+        <v>664</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D8" s="33" t="b">
         <v>1</v>
@@ -7737,13 +7701,13 @@
     </row>
     <row r="9" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>638</v>
+        <v>665</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>638</v>
+        <v>665</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D9" s="33" t="b">
         <v>1</v>
@@ -7756,13 +7720,13 @@
     </row>
     <row r="10" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>639</v>
+        <v>666</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>639</v>
+        <v>666</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D10" s="33" t="b">
         <v>1</v>
@@ -7775,13 +7739,13 @@
     </row>
     <row r="11" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>640</v>
+        <v>667</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>640</v>
+        <v>667</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D11" s="33" t="b">
         <v>1</v>
@@ -7794,13 +7758,13 @@
     </row>
     <row r="12" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>641</v>
+        <v>668</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>641</v>
+        <v>668</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D12" s="33" t="b">
         <v>1</v>
@@ -7813,13 +7777,13 @@
     </row>
     <row r="13" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>642</v>
+        <v>669</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>642</v>
+        <v>669</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D13" s="33" t="b">
         <v>1</v>
@@ -7831,13 +7795,13 @@
     </row>
     <row r="14" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>643</v>
+        <v>659</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>643</v>
+        <v>659</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D14" s="33" t="b">
         <v>1</v>
@@ -7849,13 +7813,13 @@
     </row>
     <row r="15" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
-        <v>644</v>
+        <v>670</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>644</v>
+        <v>670</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D15" s="33" t="b">
         <v>1</v>
@@ -7864,204 +7828,6 @@
         <v>207900000000</v>
       </c>
       <c r="F15" s="32"/>
-    </row>
-    <row r="16" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>645</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>645</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D16" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="32"/>
-    </row>
-    <row r="17" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>646</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>646</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D17" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="32"/>
-    </row>
-    <row r="18" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
-        <v>647</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>647</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D18" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="32"/>
-    </row>
-    <row r="19" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>648</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>648</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D19" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-    </row>
-    <row r="20" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
-        <v>649</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>649</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D20" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-    </row>
-    <row r="21" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>650</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>650</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D21" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-    </row>
-    <row r="22" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>651</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>651</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D22" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-    </row>
-    <row r="23" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D23" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-    </row>
-    <row r="24" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
-        <v>653</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>653</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D24" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
-    </row>
-    <row r="25" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
-        <v>654</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>654</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D25" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-    </row>
-    <row r="26" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33" t="s">
-        <v>655</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>655</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D26" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
-        <v>656</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>656</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="D27" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>